<commit_message>
Sửa lại model vì khóa chính và khóa ngoại không cùng data type
</commit_message>
<xml_diff>
--- a/ModelExc.xlsx
+++ b/ModelExc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hoc_tap\WebGIS\B1-Nhóm3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFA426B-94F4-4567-93EA-610F245A43D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BC4A21-3057-4C53-B5A0-1ADEAFE7EF2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD484B77-F534-4986-82CB-8DB84E246F34}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>tblUser</t>
   </si>
@@ -355,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -376,6 +376,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -690,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3661957-18E5-4C61-845D-D2109A9271D3}">
-  <dimension ref="B1:N21"/>
+  <dimension ref="B1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -904,7 +905,6 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -927,8 +927,8 @@
       <c r="G12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="6" t="s">
-        <v>16</v>
+      <c r="H12" s="20" t="s">
+        <v>1</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>28</v>
@@ -949,7 +949,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="8"/>
       <c r="H13" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="3"/>
@@ -968,7 +968,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="8"/>
       <c r="H14" s="3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="I14" s="9" t="s">
         <v>28</v>
@@ -991,7 +991,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="8"/>
       <c r="H15" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I15" s="9"/>
       <c r="J15" s="3"/>
@@ -1010,7 +1010,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="8"/>
       <c r="H16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="3"/>
@@ -1027,7 +1027,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="8"/>
       <c r="H17" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I17" s="9"/>
       <c r="J17" s="3"/>
@@ -1044,7 +1044,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="8"/>
       <c r="H18" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="3"/>
@@ -1061,7 +1061,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="8"/>
       <c r="H19" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I19" s="9"/>
       <c r="J19" s="3"/>
@@ -1076,31 +1076,48 @@
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I20" s="11"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I20" s="9"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="16"/>
     </row>
-    <row r="21" spans="2:14" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="19"/>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="15"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" s="11"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="16"/>
+    </row>
+    <row r="22" spans="2:14" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>